<commit_message>
fix tests and r check
</commit_message>
<xml_diff>
--- a/inst/concepts/PPS_concepts.xlsx
+++ b/inst/concepts/PPS_concepts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpoliti/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ablack/darwin/PregnancyIdentifier/inst/concepts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF5BE9C-CB78-0643-B4A9-ACB8A2360FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6DD867-D299-5245-86C6-6B37AEAB0836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="780" windowWidth="25300" windowHeight="18940" xr2:uid="{46FD3BAC-239C-EC42-AEF6-E9789FFC6F05}"/>
   </bookViews>
@@ -230,24 +230,6 @@
     <t>Uncertain viability of pregnancy</t>
   </si>
   <si>
-    <t>domain_concept_name</t>
-  </si>
-  <si>
-    <t>domain_concept_id</t>
-  </si>
-  <si>
-    <t>min_month</t>
-  </si>
-  <si>
-    <t>max_month</t>
-  </si>
-  <si>
-    <t>GT_month_midpoint</t>
-  </si>
-  <si>
-    <t>Gestational_TimeSpan_months</t>
-  </si>
-  <si>
     <t>Gestation period, 41 weeks</t>
   </si>
   <si>
@@ -393,6 +375,24 @@
   </si>
   <si>
     <t>Streptococcus agalactiae [Presence] in Vaginal fluid by Organism specific culture</t>
+  </si>
+  <si>
+    <t>pps_concept_name</t>
+  </si>
+  <si>
+    <t>pps_concept_id</t>
+  </si>
+  <si>
+    <t>pps_min_month</t>
+  </si>
+  <si>
+    <t>pps_max_month</t>
+  </si>
+  <si>
+    <t>pps_gestational_timespan_months</t>
+  </si>
+  <si>
+    <t>pps_gt_month_midpoint</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
   <dimension ref="A1:F113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,22 +836,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -916,7 +916,7 @@
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B5" s="4">
         <v>4014768</v>
@@ -956,7 +956,7 @@
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B7" s="4">
         <v>4146045</v>
@@ -996,7 +996,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B9">
         <v>4015296</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B10" s="4">
         <v>4014149</v>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B11" s="4">
         <v>4014150</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B12" s="4">
         <v>44808979</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B13" s="4">
         <v>4015141</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B14" s="4">
         <v>44808980</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B15" s="4">
         <v>4014433</v>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B16" s="4">
         <v>4014151</v>
@@ -1156,7 +1156,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B17" s="4">
         <v>44808981</v>
@@ -1176,7 +1176,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B18" s="4">
         <v>4015297</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B19" s="4">
         <v>4015298</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B20" s="4">
         <v>4014434</v>
@@ -1236,7 +1236,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B21" s="4">
         <v>4015299</v>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B22" s="4">
         <v>4015142</v>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B23" s="4">
         <v>4014152</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B24" s="4">
         <v>4015300</v>
@@ -1316,7 +1316,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B25" s="4">
         <v>4015301</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B26" s="4">
         <v>4015302</v>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B27" s="4">
         <v>4014435</v>
@@ -1376,7 +1376,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B28" s="4">
         <v>4143646</v>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B29" s="4">
         <v>40479665</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B31" s="4">
         <v>46273020</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="37" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B37" s="4">
         <v>4290009</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="38" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B38" s="4">
         <v>4313026</v>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B39" s="4">
         <v>4270513</v>
@@ -1716,7 +1716,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B45" s="4">
         <v>4181468</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B47" s="4">
         <v>4178165</v>
@@ -1876,7 +1876,7 @@
     </row>
     <row r="53" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B53" s="4">
         <v>4324063</v>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B58" s="4">
         <v>439922</v>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B75">
         <v>442769</v>
@@ -2336,7 +2336,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B76">
         <v>444067</v>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B78" s="4">
         <v>4245908</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B85" s="4">
         <v>3174212</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="86" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B86" s="4">
         <v>4336958</v>
@@ -2596,7 +2596,7 @@
     </row>
     <row r="89" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B89" s="4">
         <v>4041878</v>
@@ -2676,7 +2676,7 @@
     </row>
     <row r="93" spans="1:6" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B93" s="4">
         <v>3020321</v>
@@ -2736,7 +2736,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B96" s="4">
         <v>4180111</v>
@@ -2796,7 +2796,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B99" s="4">
         <v>3050401</v>
@@ -2816,7 +2816,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B100" s="4">
         <v>36303380</v>
@@ -2836,7 +2836,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B101" s="4">
         <v>40770418</v>
@@ -2856,7 +2856,7 @@
     </row>
     <row r="102" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B102" s="4">
         <v>3052868</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B103" s="4">
         <v>3049207</v>
@@ -2996,7 +2996,7 @@
     </row>
     <row r="109" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B109" s="4">
         <v>3657563</v>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="110" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B110" s="4">
         <v>4252252</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="111" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B111" s="4">
         <v>4327745</v>
@@ -3056,7 +3056,7 @@
     </row>
     <row r="112" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B112" s="4">
         <v>40486918</v>
@@ -3073,7 +3073,7 @@
     </row>
     <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B113" s="4">
         <v>2793349</v>

</xml_diff>